<commit_message>
updated Iteration 2 hours and burndown chart
</commit_message>
<xml_diff>
--- a/Project Hours Tracking.xlsx
+++ b/Project Hours Tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/830fdde6c338a896/Documents/IST 303/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{043C9774-781E-4767-AF5C-F0A713E03DE8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{0C88941A-F608-4639-8F94-8FEC04286EE7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{553749E5-430E-46A0-9183-FADC114B36BD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="71">
   <si>
     <t>Milestone</t>
   </si>
@@ -247,6 +247,9 @@
   <si>
     <t>Part D - 12/11</t>
   </si>
+  <si>
+    <t>MILESTONE</t>
+  </si>
 </sst>
 </file>
 
@@ -367,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -420,10 +423,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -868,7 +874,7 @@
                   <c:v>46.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46.05</c:v>
+                  <c:v>37.799999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1942,8 +1948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G7:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1999,10 +2005,10 @@
       <c r="C2" s="3">
         <v>1</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="22">
         <v>43739</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="22" t="s">
         <v>67</v>
       </c>
       <c r="F2" s="6">
@@ -2049,10 +2055,10 @@
       <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="22">
         <v>43739</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="22" t="s">
         <v>67</v>
       </c>
       <c r="F3" s="4">
@@ -2099,10 +2105,10 @@
       <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="22">
         <v>43739</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="22" t="s">
         <v>67</v>
       </c>
       <c r="F4" s="1">
@@ -2149,10 +2155,10 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="22">
         <v>43739</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="22" t="s">
         <v>67</v>
       </c>
       <c r="F5" s="1">
@@ -2199,10 +2205,10 @@
       <c r="C6" s="3">
         <v>1</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="22">
         <v>43739</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="22" t="s">
         <v>67</v>
       </c>
       <c r="F6" s="4">
@@ -2249,16 +2255,18 @@
       <c r="C7" s="3">
         <v>2</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="22">
         <v>43753</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="22" t="s">
         <v>68</v>
       </c>
       <c r="F7" s="8">
         <v>1</v>
       </c>
-      <c r="G7" s="8"/>
+      <c r="G7" s="8">
+        <v>0.5</v>
+      </c>
       <c r="H7" s="9" t="s">
         <v>13</v>
       </c>
@@ -2297,16 +2305,18 @@
       <c r="C8" s="3">
         <v>2</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="22">
         <v>43753</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="22" t="s">
         <v>68</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1">
+        <v>0.25</v>
+      </c>
       <c r="H8" s="9" t="s">
         <v>13</v>
       </c>
@@ -2345,16 +2355,18 @@
       <c r="C9" s="3">
         <v>2</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="22">
         <v>43753</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="22" t="s">
         <v>68</v>
       </c>
       <c r="F9" s="1">
         <v>0.25</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1">
+        <v>0.25</v>
+      </c>
       <c r="H9" s="9" t="s">
         <v>13</v>
       </c>
@@ -2393,16 +2405,18 @@
       <c r="C10" s="3">
         <v>2</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="22">
         <v>43753</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="22" t="s">
         <v>68</v>
       </c>
       <c r="F10" s="1">
         <v>4</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1">
+        <v>6.75</v>
+      </c>
       <c r="H10" s="9" t="s">
         <v>13</v>
       </c>
@@ -2441,16 +2455,18 @@
       <c r="C11" s="3">
         <v>2</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="22">
         <v>43753</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="22" t="s">
         <v>68</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1">
+        <v>0.5</v>
+      </c>
       <c r="H11" s="9" t="s">
         <v>13</v>
       </c>
@@ -2489,10 +2505,10 @@
       <c r="C12" s="3">
         <v>3</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="22">
         <v>43767</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="22" t="s">
         <v>68</v>
       </c>
       <c r="F12" s="8">
@@ -2537,10 +2553,10 @@
       <c r="C13" s="3">
         <v>3</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="22">
         <v>43767</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="22" t="s">
         <v>68</v>
       </c>
       <c r="F13" s="8">
@@ -2585,10 +2601,10 @@
       <c r="C14" s="3">
         <v>3</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="22">
         <v>43767</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="22" t="s">
         <v>68</v>
       </c>
       <c r="F14" s="8">
@@ -2633,10 +2649,10 @@
       <c r="C15" s="3">
         <v>3</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="22">
         <v>43767</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="22" t="s">
         <v>68</v>
       </c>
       <c r="F15" s="8">
@@ -2681,10 +2697,10 @@
       <c r="C16" s="3">
         <v>3</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="22">
         <v>43767</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="E16" s="22" t="s">
         <v>68</v>
       </c>
       <c r="F16" s="8">
@@ -2729,10 +2745,10 @@
       <c r="C17" s="3">
         <v>3</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="22">
         <v>43767</v>
       </c>
-      <c r="E17" s="23" t="s">
+      <c r="E17" s="22" t="s">
         <v>68</v>
       </c>
       <c r="F17" s="8">
@@ -2777,10 +2793,10 @@
       <c r="C18" s="3">
         <v>3</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="22">
         <v>43767</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="22" t="s">
         <v>68</v>
       </c>
       <c r="F18" s="8">
@@ -2825,10 +2841,10 @@
       <c r="C19" s="3">
         <v>4</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="22">
         <v>43781</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F19" s="8">
@@ -2873,10 +2889,10 @@
       <c r="C20" s="3">
         <v>4</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="22">
         <v>43781</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F20" s="8">
@@ -2921,10 +2937,10 @@
       <c r="C21" s="3">
         <v>4</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D21" s="22">
         <v>43781</v>
       </c>
-      <c r="E21" s="23" t="s">
+      <c r="E21" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F21" s="8">
@@ -2969,10 +2985,10 @@
       <c r="C22" s="3">
         <v>4</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="22">
         <v>43781</v>
       </c>
-      <c r="E22" s="23" t="s">
+      <c r="E22" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F22" s="8">
@@ -3017,10 +3033,10 @@
       <c r="C23" s="3">
         <v>4</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D23" s="22">
         <v>43781</v>
       </c>
-      <c r="E23" s="23" t="s">
+      <c r="E23" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F23" s="8">
@@ -3065,10 +3081,10 @@
       <c r="C24" s="3">
         <v>4</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="22">
         <v>43781</v>
       </c>
-      <c r="E24" s="23" t="s">
+      <c r="E24" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F24" s="8">
@@ -3113,10 +3129,10 @@
       <c r="C25" s="3">
         <v>4</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="22">
         <v>43781</v>
       </c>
-      <c r="E25" s="23" t="s">
+      <c r="E25" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F25" s="8">
@@ -3161,10 +3177,10 @@
       <c r="C26" s="3">
         <v>5</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="22">
         <v>43795</v>
       </c>
-      <c r="E26" s="23" t="s">
+      <c r="E26" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F26" s="8">
@@ -3209,10 +3225,10 @@
       <c r="C27" s="3">
         <v>5</v>
       </c>
-      <c r="D27" s="23">
+      <c r="D27" s="22">
         <v>43795</v>
       </c>
-      <c r="E27" s="23" t="s">
+      <c r="E27" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F27" s="8">
@@ -3257,10 +3273,10 @@
       <c r="C28" s="3">
         <v>5</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="22">
         <v>43795</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F28" s="8">
@@ -3305,10 +3321,10 @@
       <c r="C29" s="3">
         <v>5</v>
       </c>
-      <c r="D29" s="23">
+      <c r="D29" s="22">
         <v>43795</v>
       </c>
-      <c r="E29" s="23" t="s">
+      <c r="E29" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F29" s="8">
@@ -3353,10 +3369,10 @@
       <c r="C30" s="3">
         <v>5</v>
       </c>
-      <c r="D30" s="23">
+      <c r="D30" s="22">
         <v>43795</v>
       </c>
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F30" s="8">
@@ -3401,10 +3417,10 @@
       <c r="C31" s="3">
         <v>5</v>
       </c>
-      <c r="D31" s="23">
+      <c r="D31" s="22">
         <v>43795</v>
       </c>
-      <c r="E31" s="23" t="s">
+      <c r="E31" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F31" s="8">
@@ -3449,10 +3465,10 @@
       <c r="C32" s="3">
         <v>5</v>
       </c>
-      <c r="D32" s="23">
+      <c r="D32" s="22">
         <v>43795</v>
       </c>
-      <c r="E32" s="23" t="s">
+      <c r="E32" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F32" s="8">
@@ -3497,10 +3513,10 @@
       <c r="C33" s="3">
         <v>6</v>
       </c>
-      <c r="D33" s="23">
+      <c r="D33" s="22">
         <v>43809</v>
       </c>
-      <c r="E33" s="23" t="s">
+      <c r="E33" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F33" s="8">
@@ -3545,10 +3561,10 @@
       <c r="C34" s="3">
         <v>6</v>
       </c>
-      <c r="D34" s="23">
+      <c r="D34" s="22">
         <v>43809</v>
       </c>
-      <c r="E34" s="23" t="s">
+      <c r="E34" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F34" s="8">
@@ -3593,10 +3609,10 @@
       <c r="C35" s="3">
         <v>6</v>
       </c>
-      <c r="D35" s="23">
+      <c r="D35" s="22">
         <v>43809</v>
       </c>
-      <c r="E35" s="23" t="s">
+      <c r="E35" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F35" s="8">
@@ -3641,10 +3657,10 @@
       <c r="C36" s="3">
         <v>6</v>
       </c>
-      <c r="D36" s="23">
+      <c r="D36" s="22">
         <v>43809</v>
       </c>
-      <c r="E36" s="23" t="s">
+      <c r="E36" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F36" s="8">
@@ -3689,10 +3705,10 @@
       <c r="C37" s="3">
         <v>6</v>
       </c>
-      <c r="D37" s="23">
+      <c r="D37" s="22">
         <v>43809</v>
       </c>
-      <c r="E37" s="23" t="s">
+      <c r="E37" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F37" s="8">
@@ -3737,10 +3753,10 @@
       <c r="C38" s="3">
         <v>6</v>
       </c>
-      <c r="D38" s="23">
+      <c r="D38" s="22">
         <v>43809</v>
       </c>
-      <c r="E38" s="23" t="s">
+      <c r="E38" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F38" s="8">
@@ -3785,10 +3801,10 @@
       <c r="C39" s="3">
         <v>6</v>
       </c>
-      <c r="D39" s="23">
+      <c r="D39" s="22">
         <v>43809</v>
       </c>
-      <c r="E39" s="23" t="s">
+      <c r="E39" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F39" s="8">
@@ -3833,10 +3849,10 @@
       <c r="C40" s="3">
         <v>6</v>
       </c>
-      <c r="D40" s="23">
+      <c r="D40" s="22">
         <v>43809</v>
       </c>
-      <c r="E40" s="23" t="s">
+      <c r="E40" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F40" s="8">
@@ -34989,8 +35005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{536CEB81-96EC-49BA-953F-45D5ED1ACFD7}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -34999,16 +35015,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
@@ -35080,7 +35096,7 @@
       </c>
       <c r="D4" s="18">
         <f>(SUMIF('Base data'!C:C,2,'Base data'!G:G))</f>
-        <v>0</v>
+        <v>8.25</v>
       </c>
       <c r="E4" s="18">
         <f>(SUMIF('Base data'!C:C,3,'Base data'!G:G))</f>
@@ -35100,16 +35116,16 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
     </row>
     <row r="7" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
@@ -35143,27 +35159,27 @@
         <v>50.25</v>
       </c>
       <c r="C8" s="20">
-        <f>B8-C3</f>
+        <f t="shared" ref="C8:H8" si="0">B8-C3</f>
         <v>43</v>
       </c>
       <c r="D8" s="20">
-        <f>C8-D3</f>
+        <f t="shared" si="0"/>
         <v>35.75</v>
       </c>
       <c r="E8" s="20">
-        <f>D8-E3</f>
+        <f t="shared" si="0"/>
         <v>27.5</v>
       </c>
       <c r="F8" s="20">
-        <f>E8-F3</f>
+        <f t="shared" si="0"/>
         <v>17.75</v>
       </c>
       <c r="G8" s="20">
-        <f>F8-G3</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="H8" s="20">
-        <f>G8-H3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -35180,7 +35196,7 @@
       </c>
       <c r="D9" s="18">
         <f>C9-D4</f>
-        <v>46.05</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
@@ -35199,71 +35215,93 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B36554-C903-4683-AC14-0271685C13BE}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="130" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.3984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="87.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.796875" customWidth="1"/>
+    <col min="2" max="2" width="10.3984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="87.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12">
+        <v>1</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="C4" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12">
         <v>4</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="C5" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
+        <v>2</v>
+      </c>
+      <c r="B6" s="12">
         <v>5</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="C6" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
+        <v>2</v>
+      </c>
+      <c r="B7" s="12">
         <v>6</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="C7" s="13" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>